<commit_message>
charlson inspq + manitoba
</commit_message>
<xml_diff>
--- a/inst/extdata/Comorbidity_weights.xlsx
+++ b/inst/extdata/Comorbidity_weights.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\INESSS-QC_inesss1\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317134A6-3688-41CA-8123-A8F8CD8FE01C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE68788-FFB8-4A0A-9A84-13E784E30124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28125" yWindow="885" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CCI_INSPQ_2018_CIM9" sheetId="1" r:id="rId1"/>
     <sheet name="CCI_INSPQ_2018_CIM10" sheetId="3" r:id="rId2"/>
     <sheet name="UManitoba_2016" sheetId="2" r:id="rId3"/>
+    <sheet name="CCI_INSPQ_Manitoba" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="92">
   <si>
     <t>Hypertension</t>
   </si>
@@ -635,7 +636,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,7 +1056,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A32" sqref="A32:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,8 +1438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0703C3A3-1F1A-4B7D-B1DE-D3C78DAA3646}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,32 +1462,254 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>70</v>
       </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C18">
+    <sortCondition ref="B2:B18"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8D7742-BCF3-415C-BAB7-1B1965986418}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1505,10 +1728,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1549,76 +1772,76 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1626,10 +1849,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1637,18 +1860,18 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C18">
-    <sortCondition ref="A2:A18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C17">
+    <sortCondition ref="B2:B17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>